<commit_message>
Versión 1 - ISPEL Beta 2024 para fabricar (corregido).
</commit_message>
<xml_diff>
--- a/Docs/Listado de materiales ISPEL.xlsx
+++ b/Docs/Listado de materiales ISPEL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gcapo\Repositorios\gcapora\ISPEL-CAD\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ADB0F73-4F83-499B-9D04-2E2C36B20CE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65CE4C0E-F819-432B-9954-B037115EA60E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-1815" windowWidth="28080" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ISPEL-CAD_v1 (5)" sheetId="6" r:id="rId1"/>

</xml_diff>